<commit_message>
added stuff on plant viruses
</commit_message>
<xml_diff>
--- a/Documents/qPCR_Setup_Files/Plate setup template for 1step qPCR.xlsx
+++ b/Documents/qPCR_Setup_Files/Plate setup template for 1step qPCR.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="93">
   <si>
     <t>DWV</t>
   </si>
@@ -617,10 +617,22 @@
     </r>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>G-block</t>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>-7</t>
+  </si>
+  <si>
+    <t>-5</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>Gblock</t>
+  </si>
+  <si>
+    <t>-7raw</t>
   </si>
 </sst>
 </file>
@@ -858,8 +870,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="245">
+  <cellStyleXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1286,7 +1300,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="245">
+  <cellStyles count="247">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1409,6 +1423,7 @@
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1531,6 +1546,7 @@
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2375,7 +2391,7 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2467,11 +2483,21 @@
       <c r="B2" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -2511,12 +2537,24 @@
       <c r="A3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -2557,20 +2595,28 @@
       <c r="A4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="9" t="s">
-        <v>88</v>
-      </c>
+      <c r="M4" s="9"/>
       <c r="N4" s="46" t="s">
         <v>0</v>
       </c>
@@ -2608,12 +2654,8 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
-      <c r="M5" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="46" t="s">
-        <v>0</v>
-      </c>
+      <c r="M5" s="55"/>
+      <c r="N5" s="46"/>
       <c r="P5" s="31">
         <v>16600000000</v>
       </c>
@@ -2655,9 +2697,7 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="65" t="s">
-        <v>59</v>
-      </c>
+      <c r="N6" s="65"/>
       <c r="O6" s="2"/>
       <c r="P6" s="31">
         <v>42500000000</v>
@@ -2700,9 +2740,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="65" t="s">
-        <v>59</v>
-      </c>
+      <c r="N7" s="65"/>
       <c r="O7" s="2"/>
       <c r="P7" s="28">
         <v>25100000000</v>
@@ -2744,12 +2782,8 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="N8" s="65" t="s">
-        <v>59</v>
-      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="2"/>
       <c r="P8" s="33">
         <v>74300000000</v>
@@ -2791,12 +2825,8 @@
       <c r="J9" s="45"/>
       <c r="K9" s="45"/>
       <c r="L9" s="45"/>
-      <c r="M9" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="65" t="s">
-        <v>59</v>
-      </c>
+      <c r="M9" s="55"/>
+      <c r="N9" s="65"/>
       <c r="O9" s="2"/>
       <c r="P9" s="30">
         <v>83200000000</v>

</xml_diff>